<commit_message>
Adding plot of general results
</commit_message>
<xml_diff>
--- a/Paths.xlsx
+++ b/Paths.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\loren\Documents\GitHub\SESAM\GT-IOA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nicog\Desktop\Nicolò\GitHub\GreenTechs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67F1C511-F6E4-4BF5-9774-6A28EEDAD009}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F1B153E-6909-4950-BFA3-FD5262A7A5BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="26">
   <si>
     <t>LR</t>
   </si>
@@ -36,52 +36,73 @@
     <t>Database</t>
   </si>
   <si>
-    <t>C:\Users\loren\Documents\GitHub\SESAM\GT-IOA\Database</t>
-  </si>
-  <si>
-    <t>C:\Users\loren\Documents\GitHub\SESAM\GT-IOA\Shocks</t>
-  </si>
-  <si>
     <t>EXIOBASE SUT</t>
   </si>
   <si>
     <t>EXIOBASE IOT</t>
   </si>
   <si>
-    <t>C:\Users\loren\Documents\GitHub\SESAM\GT-IOA\Add sectors</t>
-  </si>
-  <si>
     <t>Add Sectors</t>
   </si>
   <si>
     <t>Shocks</t>
   </si>
   <si>
-    <t>C:\Users\loren\Documents\GitHub\SESAM\GT-IOA\Results</t>
-  </si>
-  <si>
     <t>Plots</t>
   </si>
   <si>
-    <t>C:\Users\loren\Documents\GitHub\SESAM\GT-IOA\Plots</t>
-  </si>
-  <si>
-    <t>C:\Users\loren\Politecnico di Milano\DENG-SESAM - Documenti\DATASETS\Exiobase Hybrid 3.3.18</t>
-  </si>
-  <si>
     <t>EXIOBASE Hybrid</t>
   </si>
   <si>
-    <t>C:\Users\loren\Politecnico di Milano\DENG-SESAM - Documenti\DATASETS\Exiobase 3.8.2\MRSUT</t>
-  </si>
-  <si>
-    <t>C:\Users\loren\Politecnico di Milano\DENG-SESAM - Documenti\DATASETS\Exiobase 3.8.2\IOT</t>
-  </si>
-  <si>
-    <t>C:\Users\loren\Documents\GitHub\SESAM\GT-IOA\Shocks\ShockMaster.xlsx</t>
-  </si>
-  <si>
     <t>ShockMaster</t>
+  </si>
+  <si>
+    <t>C:\Users\nicog\Documents\GitHub\SESAM\GT-IOA\Database</t>
+  </si>
+  <si>
+    <t>C:\Users\nicog\Documents\GitHub\SESAM\GT-IOA\Add sectors</t>
+  </si>
+  <si>
+    <t>C:\Users\nicog\Documents\GitHub\SESAM\GT-IOA\Shocks</t>
+  </si>
+  <si>
+    <t>C:\Users\nicog\Documents\GitHub\SESAM\GT-IOA\Results</t>
+  </si>
+  <si>
+    <t>C:\Users\nicog\Documents\GitHub\SESAM\GT-IOA\Plots</t>
+  </si>
+  <si>
+    <t>C:\Users\nicog\Documents\GitHub\SESAM\GT-IOA\Shocks\ShockMaster.xlsx</t>
+  </si>
+  <si>
+    <t>C:\Users\nicog\Politecnico di Milano\DENG-SESAM - Documenti\DATASETS\Exiobase 3.8.2\MRSUT</t>
+  </si>
+  <si>
+    <t>C:\Users\nicog\Politecnico di Milano\DENG-SESAM - Documenti\DATASETS\Exiobase 3.8.2\IOT</t>
+  </si>
+  <si>
+    <t>C:\Users\nicog\Politecnico di Milano\DENG-SESAM - Documenti\DATASETS\Exiobase Hybrid 3.3.18</t>
+  </si>
+  <si>
+    <t>C:\Users\nicog\Desktop\Nicolò\GitHub\GreenTechs\Database</t>
+  </si>
+  <si>
+    <t>C:\Users\nicog\Desktop\Nicolò\GitHub\GreenTechs\Add sectors</t>
+  </si>
+  <si>
+    <t>C:\Users\nicog\Desktop\Nicolò\GitHub\GreenTechs\Shocks</t>
+  </si>
+  <si>
+    <t>C:\Users\nicog\Desktop\Nicolò\GitHub\GreenTechs\Results</t>
+  </si>
+  <si>
+    <t>C:\Users\nicog\Desktop\Nicolò\GitHub\GreenTechs\Plots</t>
+  </si>
+  <si>
+    <t>C:\Users\nicog\Desktop\Nicolò\GitHub\GreenTechs\ShockMaster.xlsx</t>
+  </si>
+  <si>
+    <t>NG</t>
   </si>
 </sst>
 </file>
@@ -122,7 +143,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normale" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -400,93 +421,123 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="105.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="105.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+      <c r="C2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+      <c r="C3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+      <c r="C4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+      <c r="C5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+      <c r="C6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="C7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>1</v>
       </c>
       <c r="B8" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+      <c r="C8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+      <c r="C9" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>17</v>
+        <v>15</v>
+      </c>
+      <c r="C10" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changed paths for LR
</commit_message>
<xml_diff>
--- a/Paths.xlsx
+++ b/Paths.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nicog\Desktop\Nicolò\GitHub\GreenTechs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\loren\Documents\GitHub\MARIO Organization\GreenTechs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F1B153E-6909-4950-BFA3-FD5262A7A5BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84896273-4BB5-4DC4-A36E-AAC383E2AF28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>LR</t>
   </si>
@@ -57,24 +57,6 @@
     <t>ShockMaster</t>
   </si>
   <si>
-    <t>C:\Users\nicog\Documents\GitHub\SESAM\GT-IOA\Database</t>
-  </si>
-  <si>
-    <t>C:\Users\nicog\Documents\GitHub\SESAM\GT-IOA\Add sectors</t>
-  </si>
-  <si>
-    <t>C:\Users\nicog\Documents\GitHub\SESAM\GT-IOA\Shocks</t>
-  </si>
-  <si>
-    <t>C:\Users\nicog\Documents\GitHub\SESAM\GT-IOA\Results</t>
-  </si>
-  <si>
-    <t>C:\Users\nicog\Documents\GitHub\SESAM\GT-IOA\Plots</t>
-  </si>
-  <si>
-    <t>C:\Users\nicog\Documents\GitHub\SESAM\GT-IOA\Shocks\ShockMaster.xlsx</t>
-  </si>
-  <si>
     <t>C:\Users\nicog\Politecnico di Milano\DENG-SESAM - Documenti\DATASETS\Exiobase 3.8.2\MRSUT</t>
   </si>
   <si>
@@ -103,6 +85,33 @@
   </si>
   <si>
     <t>NG</t>
+  </si>
+  <si>
+    <t>C:\Users\loren\Politecnico di Milano\DENG-SESAM - Documenti\DATASETS\Exiobase 3.8.2\MRSUT</t>
+  </si>
+  <si>
+    <t>C:\Users\loren\Politecnico di Milano\DENG-SESAM - Documenti\DATASETS\Exiobase 3.8.2\IOT</t>
+  </si>
+  <si>
+    <t>C:\Users\loren\Politecnico di Milano\DENG-SESAM - Documenti\DATASETS\Exiobase Hybrid 3.3.18</t>
+  </si>
+  <si>
+    <t>C:\Users\loren\Documents\GitHub\MARIO Organization\GreenTechs\Database</t>
+  </si>
+  <si>
+    <t>C:\Users\loren\Documents\GitHub\MARIO Organization\GreenTechs\Add sectors</t>
+  </si>
+  <si>
+    <t>C:\Users\loren\Documents\GitHub\MARIO Organization\GreenTechs\Shocks</t>
+  </si>
+  <si>
+    <t>C:\Users\loren\Documents\GitHub\MARIO Organization\GreenTechs\Results</t>
+  </si>
+  <si>
+    <t>C:\Users\loren\Documents\GitHub\MARIO Organization\GreenTechs\Plots</t>
+  </si>
+  <si>
+    <t>C:\Users\loren\Documents\GitHub\MARIO Organization\GreenTechs\Shocks\ShockMaster.xlsx</t>
   </si>
 </sst>
 </file>
@@ -424,7 +433,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -438,7 +447,7 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -446,10 +455,10 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C2" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -457,10 +466,10 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C3" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -468,10 +477,10 @@
         <v>8</v>
       </c>
       <c r="B4" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="C4" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -479,10 +488,10 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="C5" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -490,10 +499,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="C6" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
@@ -501,10 +510,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="C7" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
@@ -512,10 +521,10 @@
         <v>1</v>
       </c>
       <c r="B8" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="C8" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
@@ -523,10 +532,10 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>14</v>
+        <v>27</v>
       </c>
       <c r="C9" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
@@ -534,10 +543,10 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="C10" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
saved databases with new sectors
</commit_message>
<xml_diff>
--- a/Paths.xlsx
+++ b/Paths.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\loren\Documents\GitHub\MARIO Organization\GreenTechs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84896273-4BB5-4DC4-A36E-AAC383E2AF28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B6D874A-2E2A-42DC-9DED-65F779736DD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -436,13 +436,13 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="105.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="105.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -450,7 +450,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -461,7 +461,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -472,7 +472,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
@@ -483,7 +483,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -494,7 +494,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -505,7 +505,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -516,7 +516,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>1</v>
       </c>
@@ -527,7 +527,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -538,7 +538,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>

</xml_diff>

<commit_message>
changed LR paths and fixed regions of add commodities
</commit_message>
<xml_diff>
--- a/Paths.xlsx
+++ b/Paths.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://polimi365-my.sharepoint.com/personal/10608728_polimi_it/Documents/Documenti/GitHub/GreenTechs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\loren\Documents\GitHub\SESAM\GreenTechs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="16" documentId="13_ncr:1_{67D918D9-7CD6-40B8-8319-60D6D52531FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B767FE43-74E1-4DC8-92A6-EB7AC83B4D66}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3555A7F-78A0-48CD-A3DC-0A55822CAC9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="15260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -93,24 +93,6 @@
     <t>C:\Users\loren\Politecnico di Milano\DENG-SESAM - Documenti\DATASETS\Exiobase Hybrid 3.3.18</t>
   </si>
   <si>
-    <t>C:\Users\loren\Documents\GitHub\MARIO Organization\GreenTechs\Database</t>
-  </si>
-  <si>
-    <t>C:\Users\loren\Documents\GitHub\MARIO Organization\GreenTechs\Add sectors</t>
-  </si>
-  <si>
-    <t>C:\Users\loren\Documents\GitHub\MARIO Organization\GreenTechs\Shocks</t>
-  </si>
-  <si>
-    <t>C:\Users\loren\Documents\GitHub\MARIO Organization\GreenTechs\Results</t>
-  </si>
-  <si>
-    <t>C:\Users\loren\Documents\GitHub\MARIO Organization\GreenTechs\Plots</t>
-  </si>
-  <si>
-    <t>C:\Users\loren\Documents\GitHub\MARIO Organization\GreenTechs\Shocks\ShockMaster.xlsx</t>
-  </si>
-  <si>
     <t>C:\Users\nicog\Desktop\Nicolò\GitHub\GreenTechs\Shocks\ShockMaster.xlsx</t>
   </si>
   <si>
@@ -169,6 +151,24 @@
   </si>
   <si>
     <t>C:\Users\matti\OneDrive - Politecnico di Milano\Documenti\GitHub\GreenTechs\Shocks\ShockMaster.xlsx</t>
+  </si>
+  <si>
+    <t>C:\Users\loren\Documents\GitHub\SESAM\GreenTechs\Database</t>
+  </si>
+  <si>
+    <t>C:\Users\loren\Documents\GitHub\SESAM\GreenTechs\Add sectors</t>
+  </si>
+  <si>
+    <t>C:\Users\loren\Documents\GitHub\SESAM\GreenTechs\Shocks</t>
+  </si>
+  <si>
+    <t>C:\Users\loren\Documents\GitHub\SESAM\GreenTechs\Results</t>
+  </si>
+  <si>
+    <t>C:\Users\loren\Documents\GitHub\SESAM\GreenTechs\Plots</t>
+  </si>
+  <si>
+    <t>C:\Users\loren\Documents\GitHub\SESAM\GreenTechs\Shocks\ShockMaster.xlsx</t>
   </si>
 </sst>
 </file>
@@ -489,18 +489,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="105.6328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="84.36328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="105.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="84.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -508,13 +508,13 @@
         <v>18</v>
       </c>
       <c r="D1" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="E1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -525,13 +525,13 @@
         <v>10</v>
       </c>
       <c r="D2" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="E2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -542,13 +542,13 @@
         <v>11</v>
       </c>
       <c r="D3" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="E3" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
@@ -559,109 +559,109 @@
         <v>12</v>
       </c>
       <c r="E4" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>22</v>
+        <v>42</v>
       </c>
       <c r="C5" t="s">
         <v>13</v>
       </c>
       <c r="D5" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="E5" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>23</v>
+        <v>43</v>
       </c>
       <c r="C6" t="s">
         <v>14</v>
       </c>
       <c r="D6" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="E6" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>24</v>
+        <v>44</v>
       </c>
       <c r="C7" t="s">
         <v>15</v>
       </c>
       <c r="D7" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="E7" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>1</v>
       </c>
       <c r="B8" t="s">
-        <v>25</v>
+        <v>45</v>
       </c>
       <c r="C8" t="s">
         <v>16</v>
       </c>
       <c r="D8" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="E8" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>26</v>
+        <v>46</v>
       </c>
       <c r="C9" t="s">
         <v>17</v>
       </c>
       <c r="D9" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="E9" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>27</v>
+        <v>47</v>
       </c>
       <c r="C10" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="D10" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="E10" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
something put in old and shock on intermediate consumption of crms implemented. baseline database done
</commit_message>
<xml_diff>
--- a/Paths.xlsx
+++ b/Paths.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\loren\Documents\GitHub\SESAM\GreenTechs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3555A7F-78A0-48CD-A3DC-0A55822CAC9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68D9DB9D-D0EA-453E-85AC-CAE3305999C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
   <si>
     <t>LR</t>
   </si>
@@ -169,6 +169,12 @@
   </si>
   <si>
     <t>C:\Users\loren\Documents\GitHub\SESAM\GreenTechs\Shocks\ShockMaster.xlsx</t>
+  </si>
+  <si>
+    <t>CRMs shock data</t>
+  </si>
+  <si>
+    <t>C:\Users\loren\Documents\GitHub\SESAM\GreenTechs\Support data\CRMs shocks.xlsx</t>
   </si>
 </sst>
 </file>
@@ -487,10 +493,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -664,6 +670,14 @@
         <v>41</v>
       </c>
     </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>48</v>
+      </c>
+      <c r="B11" t="s">
+        <v>49</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Added code 4. for making the SUT an IOT; in order to make the IOT a WIOT waste sectors and waste types are added
Note: the waste types and sectors need to be checked
</commit_message>
<xml_diff>
--- a/Paths.xlsx
+++ b/Paths.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\loren\Documents\GitHub\SESAM\GreenTechs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\carol\OneDrive\Documenti\GitHub\GreenTechs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68D9DB9D-D0EA-453E-85AC-CAE3305999C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6C8BE96-8C6D-4979-9FB2-A7769E0BD6AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
   <si>
     <t>LR</t>
   </si>
@@ -102,24 +102,6 @@
     <t>C:\Users\carol\Desktop\UNI\MAGISTRALE\TESI\IOT</t>
   </si>
   <si>
-    <t>C:\Users\carol\Desktop\UNI\MAGISTRALE\TESI\GitHub\GreenTechs\Database</t>
-  </si>
-  <si>
-    <t>C:\Users\carol\Desktop\UNI\MAGISTRALE\TESI\GitHub\GreenTechs\Add Sectors</t>
-  </si>
-  <si>
-    <t>C:\Users\carol\Desktop\UNI\MAGISTRALE\TESI\GitHub\GreenTechs\Shocks</t>
-  </si>
-  <si>
-    <t>C:\Users\carol\Desktop\UNI\MAGISTRALE\TESI\GitHub\GreenTechs\Results</t>
-  </si>
-  <si>
-    <t>C:\Users\carol\Desktop\UNI\MAGISTRALE\TESI\GitHub\GreenTechs\Plots</t>
-  </si>
-  <si>
-    <t>C:\Users\carol\Desktop\UNI\MAGISTRALE\TESI\GitHub\GreenTechs\Shocks\ShockMaster.xlsx</t>
-  </si>
-  <si>
     <t>C:\Users\carol\Desktop\UNI\MAGISTRALE\TESI\MRSUT</t>
   </si>
   <si>
@@ -175,6 +157,27 @@
   </si>
   <si>
     <t>C:\Users\loren\Documents\GitHub\SESAM\GreenTechs\Support data\CRMs shocks.xlsx</t>
+  </si>
+  <si>
+    <t>C:\Users\carol\OneDrive\Documenti\GitHub\GreenTechs\Shocks\ShockMaster.xlsx</t>
+  </si>
+  <si>
+    <t>C:\Users\carol\OneDrive\Documenti\GitHub\GreenTechs\Database</t>
+  </si>
+  <si>
+    <t>C:\Users\carol\OneDrive\Documenti\GitHub\GreenTechs\Add Sectors</t>
+  </si>
+  <si>
+    <t>C:\Users\carol\OneDrive\Documenti\GitHub\GreenTechs\Shocks</t>
+  </si>
+  <si>
+    <t>C:\Users\carol\OneDrive\Documenti\GitHub\GreenTechs\Results</t>
+  </si>
+  <si>
+    <t>C:\Users\carol\OneDrive\Documenti\GitHub\GreenTechs\Plots</t>
+  </si>
+  <si>
+    <t>C:\Users\carol\OneDrive\Documenti\GitHub\GreenTechs\Add Waste Sectors</t>
   </si>
 </sst>
 </file>
@@ -493,20 +496,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="105.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="84.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="105.6328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="84.36328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="80.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -517,10 +521,10 @@
         <v>23</v>
       </c>
       <c r="E1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -531,13 +535,13 @@
         <v>10</v>
       </c>
       <c r="D2" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="E2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -551,10 +555,10 @@
         <v>24</v>
       </c>
       <c r="E3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
@@ -565,117 +569,122 @@
         <v>12</v>
       </c>
       <c r="E4" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="C5" t="s">
         <v>13</v>
       </c>
       <c r="D5" t="s">
-        <v>25</v>
+        <v>45</v>
       </c>
       <c r="E5" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C6" t="s">
         <v>14</v>
       </c>
       <c r="D6" t="s">
-        <v>26</v>
+        <v>46</v>
       </c>
       <c r="E6" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="C7" t="s">
         <v>15</v>
       </c>
       <c r="D7" t="s">
-        <v>27</v>
+        <v>47</v>
       </c>
       <c r="E7" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>1</v>
       </c>
       <c r="B8" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C8" t="s">
         <v>16</v>
       </c>
       <c r="D8" t="s">
-        <v>28</v>
+        <v>48</v>
       </c>
       <c r="E8" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="C9" t="s">
         <v>17</v>
       </c>
       <c r="D9" t="s">
-        <v>29</v>
+        <v>49</v>
       </c>
       <c r="E9" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="C10" t="s">
         <v>22</v>
       </c>
       <c r="D10" t="s">
-        <v>30</v>
+        <v>44</v>
       </c>
       <c r="E10" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="B11" t="s">
-        <v>49</v>
+        <v>43</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D12" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Creation of 5. Recycling
Calculation of EoL
Calculation of scraps
Calculation of residuals
Calculation of recycled material
Calculation of SW2 and SwFD
</commit_message>
<xml_diff>
--- a/Paths.xlsx
+++ b/Paths.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\carol\OneDrive\Documenti\GitHub\GreenTechs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://polimi365-my.sharepoint.com/personal/10421550_polimi_it/Documents/Documenti/Tesi di laurea/2022-23_WasteMARIO/dMRWIO model/dMRWIO/End of Life/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6C8BE96-8C6D-4979-9FB2-A7769E0BD6AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{6BD1CBB9-BAC5-4FC9-B618-C311FCE0B6D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4B644192-02C6-4622-92BD-64A43702D195}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="60">
   <si>
     <t>LR</t>
   </si>
@@ -177,7 +177,34 @@
     <t>C:\Users\carol\OneDrive\Documenti\GitHub\GreenTechs\Plots</t>
   </si>
   <si>
-    <t>C:\Users\carol\OneDrive\Documenti\GitHub\GreenTechs\Add Waste Sectors</t>
+    <t>fileParam</t>
+  </si>
+  <si>
+    <t>fileSolar</t>
+  </si>
+  <si>
+    <t>fileWind</t>
+  </si>
+  <si>
+    <t>C:\Users\carol\OneDrive\Documenti\GitHub\GreenTechs\Recycling\Recycling parameters.xlsx</t>
+  </si>
+  <si>
+    <t>C:\Users\carol\OneDrive\Documenti\GitHub\GreenTechs\Recycling\Solar PV Installed capacity.xlsx</t>
+  </si>
+  <si>
+    <t>C:\Users\carol\OneDrive\Documenti\GitHub\GreenTechs\Recycling\WIND Installed capacity.xlsx</t>
+  </si>
+  <si>
+    <t>SwFD</t>
+  </si>
+  <si>
+    <t>C:\Users\carol\OneDrive\Documenti\GitHub\GreenTechs\Recycling\SwFD</t>
+  </si>
+  <si>
+    <t>C:\Users\carol\OneDrive\Documenti\GitHub\GreenTechs\Recycling\SW2</t>
+  </si>
+  <si>
+    <t>SW2</t>
   </si>
 </sst>
 </file>
@@ -496,17 +523,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="105.6328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="84.36328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="2.26953125" customWidth="1"/>
     <col min="4" max="4" width="80.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -683,8 +713,43 @@
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>50</v>
+      </c>
       <c r="D12" t="s">
-        <v>50</v>
+        <v>53</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>51</v>
+      </c>
+      <c r="D13" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>52</v>
+      </c>
+      <c r="D14" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>56</v>
+      </c>
+      <c r="D15" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>59</v>
+      </c>
+      <c r="D16" t="s">
+        <v>58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Tentativo di unire in unico excel la FD
</commit_message>
<xml_diff>
--- a/Paths.xlsx
+++ b/Paths.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://polimi365-my.sharepoint.com/personal/10608728_polimi_it/Documents/Documenti/GitHub/GreenTechs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\carol\OneDrive\Documenti\GitHub\GreenTechs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{0C3E5AC3-037B-4E4F-8B87-4B21E1FFB766}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3CF51E64-A3B4-4F4E-82DD-27D812818861}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7BA5776-FD69-43B1-9EBA-249E28164791}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="15260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="85">
   <si>
     <t>LR</t>
   </si>
@@ -198,9 +198,6 @@
     <t>SwFD</t>
   </si>
   <si>
-    <t>C:\Users\carol\OneDrive\Documenti\GitHub\GreenTechs\Recycling\SwFD</t>
-  </si>
-  <si>
     <t>C:\Users\carol\OneDrive\Documenti\GitHub\GreenTechs\Recycling\SW2</t>
   </si>
   <si>
@@ -222,9 +219,6 @@
     <t>C:\Users\matti\OneDrive - Politecnico di Milano\Documenti\GitHub\GreenTechs\Recycling\WIND Installed capacity.xlsx</t>
   </si>
   <si>
-    <t>C:\Users\matti\OneDrive - Politecnico di Milano\Documenti\GitHub\GreenTechs\Recycling\SwFD</t>
-  </si>
-  <si>
     <t>C:\Users\matti\OneDrive - Politecnico di Milano\Documenti\GitHub\GreenTechs\Recycling\SW2</t>
   </si>
   <si>
@@ -252,22 +246,40 @@
     <t>C:\Users\loren\Documents\GitHub\SESAM\GreenTechs\Recycling\SG2</t>
   </si>
   <si>
-    <t>GDP projection</t>
-  </si>
-  <si>
     <t>C:\Users\carol\OneDrive\Documenti\GitHub\GreenTechs\Recycling\SG2</t>
   </si>
   <si>
-    <t>C:\Users\matti\OneDrive - Politecnico di Milano\Documenti\GitHub\GreenTechs\GDP projection\GDP projections.xlsx</t>
-  </si>
-  <si>
-    <t>C:\Users\carol\OneDrive\Documenti\GitHub\GreenTechs\GDP projection\GDP projections.xlsx</t>
-  </si>
-  <si>
     <t>AIC</t>
   </si>
   <si>
-    <t>C:\Users\matti\OneDrive - Politecnico di Milano\Documenti\GitHub\GreenTechs\Recycling\AIC</t>
+    <t>C:\Users\matti\OneDrive - Politecnico di Milano\Documenti\GitHub\GreenTechs\Final Demand\AIC</t>
+  </si>
+  <si>
+    <t>C:\Users\matti\OneDrive - Politecnico di Milano\Documenti\GitHub\GreenTechs\Final Demand\GDP projections.xlsx</t>
+  </si>
+  <si>
+    <t>C:\Users\carol\OneDrive\Documenti\GitHub\GreenTechs\Final Demand\GDP projections.xlsx</t>
+  </si>
+  <si>
+    <t>C:\Users\carol\OneDrive\Documenti\GitHub\GreenTechs\Final Demand\AIC</t>
+  </si>
+  <si>
+    <t>Projections</t>
+  </si>
+  <si>
+    <t>C:\Users\carol\OneDrive\Documenti\GitHub\GreenTechs\Final Demand\SwFD</t>
+  </si>
+  <si>
+    <t>C:\Users\matti\OneDrive - Politecnico di Milano\Documenti\GitHub\GreenTechs\Final Demand\SwFD</t>
+  </si>
+  <si>
+    <t>GDP projections</t>
+  </si>
+  <si>
+    <t>Merged FD</t>
+  </si>
+  <si>
+    <t>C:\Users\carol\OneDrive\Documenti\GitHub\GreenTechs\Final Demand</t>
   </si>
 </sst>
 </file>
@@ -592,13 +604,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="D5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E20" sqref="E20"/>
+      <selection pane="bottomRight" activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -781,10 +793,10 @@
         <v>43</v>
       </c>
       <c r="D11" t="s">
+        <v>59</v>
+      </c>
+      <c r="E11" t="s">
         <v>60</v>
-      </c>
-      <c r="E11" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
@@ -792,13 +804,13 @@
         <v>50</v>
       </c>
       <c r="B12" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D12" t="s">
         <v>53</v>
       </c>
       <c r="E12" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
@@ -806,13 +818,13 @@
         <v>51</v>
       </c>
       <c r="B13" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D13" t="s">
         <v>54</v>
       </c>
       <c r="E13" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
@@ -820,13 +832,13 @@
         <v>52</v>
       </c>
       <c r="B14" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D14" t="s">
         <v>55</v>
       </c>
       <c r="E14" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
@@ -834,60 +846,79 @@
         <v>56</v>
       </c>
       <c r="B15" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D15" t="s">
-        <v>57</v>
+        <v>80</v>
       </c>
       <c r="E15" t="s">
-        <v>65</v>
+        <v>81</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B16" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D16" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E16" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B17" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D17" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="E17" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>75</v>
+        <v>82</v>
       </c>
       <c r="D18" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E18" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
+        <v>74</v>
+      </c>
+      <c r="D19" t="s">
+        <v>78</v>
+      </c>
+      <c r="E19" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
         <v>79</v>
       </c>
-      <c r="E19" t="s">
-        <v>80</v>
+      <c r="D20" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>83</v>
+      </c>
+      <c r="D21" t="s">
+        <v>84</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Merging final demand (historical and projected separated)
</commit_message>
<xml_diff>
--- a/Paths.xlsx
+++ b/Paths.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://polimi365-my.sharepoint.com/personal/10608728_polimi_it/Documents/Documenti/GitHub/GreenTechs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\carol\OneDrive\Documenti\GitHub\GreenTechs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7" documentId="13_ncr:1_{F7BA5776-FD69-43B1-9EBA-249E28164791}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{835211DD-E40F-4E66-A6DD-D8EE6E8CE570}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{614918C7-4A52-4334-9277-CC41F083DABB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="15260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="90">
   <si>
     <t>LR</t>
   </si>
@@ -286,6 +286,15 @@
   </si>
   <si>
     <t>C:\Users\matti\OneDrive - Politecnico di Milano\Documenti\GitHub\GreenTechs\Recycling\Met_rec_comp</t>
+  </si>
+  <si>
+    <t>C:\Users\carol\OneDrive\Documenti\GitHub\GreenTechs\Recycling\Met_rec_comp</t>
+  </si>
+  <si>
+    <t>History</t>
+  </si>
+  <si>
+    <t>FD</t>
   </si>
 </sst>
 </file>
@@ -610,13 +619,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="D5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I28" sqref="I28"/>
+      <selection pane="bottomRight" activeCell="D23" sqref="D23:D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -893,6 +902,9 @@
       <c r="A18" t="s">
         <v>85</v>
       </c>
+      <c r="D18" t="s">
+        <v>87</v>
+      </c>
       <c r="E18" t="s">
         <v>86</v>
       </c>
@@ -932,6 +944,22 @@
         <v>83</v>
       </c>
       <c r="D22" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>88</v>
+      </c>
+      <c r="D23" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>89</v>
+      </c>
+      <c r="D24" t="s">
         <v>84</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Merged Historic FD and Projected FD in Total FD; MultiIndex in 6.
</commit_message>
<xml_diff>
--- a/Paths.xlsx
+++ b/Paths.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\carol\OneDrive\Documenti\GitHub\GreenTechs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{614918C7-4A52-4334-9277-CC41F083DABB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2382E260-4DA2-4786-85A1-AD1C95F2A491}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4800" yWindow="2990" windowWidth="14400" windowHeight="7810" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="94">
   <si>
     <t>LR</t>
   </si>
@@ -294,7 +294,19 @@
     <t>History</t>
   </si>
   <si>
-    <t>FD</t>
+    <t>C:\Users\carol\OneDrive\Documenti\GitHub\GreenTechs\Final Demand\Merged FD Projected</t>
+  </si>
+  <si>
+    <t>C:\Users\carol\OneDrive\Documenti\GitHub\GreenTechs\Final Demand\Total FD</t>
+  </si>
+  <si>
+    <t>Historical FD</t>
+  </si>
+  <si>
+    <t>C:\Users\carol\OneDrive\Documenti\GitHub\GreenTechs\Final Demand\Merged FD Historical</t>
+  </si>
+  <si>
+    <t>FD Total</t>
   </si>
 </sst>
 </file>
@@ -619,13 +631,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E24"/>
+  <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="D5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="D20" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D23" sqref="D23:D24"/>
+      <selection pane="bottomRight" activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -944,23 +956,31 @@
         <v>83</v>
       </c>
       <c r="D22" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="D23" t="s">
-        <v>84</v>
+        <v>92</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D24" t="s">
         <v>84</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>93</v>
+      </c>
+      <c r="D25" t="s">
+        <v>90</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Setting Final Demand Total for shock
</commit_message>
<xml_diff>
--- a/Paths.xlsx
+++ b/Paths.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\carol\OneDrive\Documenti\GitHub\GreenTechs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://polimi365-my.sharepoint.com/personal/10608728_polimi_it/Documents/Documenti/GitHub/GreenTechs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2382E260-4DA2-4786-85A1-AD1C95F2A491}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="6" documentId="13_ncr:1_{2382E260-4DA2-4786-85A1-AD1C95F2A491}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{97638154-9876-4440-BC6A-A26DB53BBABA}"/>
   <bookViews>
-    <workbookView xWindow="4800" yWindow="2990" windowWidth="14400" windowHeight="7810" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="15260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="98">
   <si>
     <t>LR</t>
   </si>
@@ -307,6 +307,18 @@
   </si>
   <si>
     <t>FD Total</t>
+  </si>
+  <si>
+    <t>C:\Users\matti\OneDrive - Politecnico di Milano\Documenti\GitHub\GreenTechs\Final Demand</t>
+  </si>
+  <si>
+    <t>C:\Users\matti\OneDrive - Politecnico di Milano\Documenti\GitHub\GreenTechs\Final Demand\Merged FD Projected</t>
+  </si>
+  <si>
+    <t>C:\Users\matti\OneDrive - Politecnico di Milano\Documenti\GitHub\GreenTechs\Final Demand\Merged FD Historical</t>
+  </si>
+  <si>
+    <t>C:\Users\matti\OneDrive - Politecnico di Milano\Documenti\GitHub\GreenTechs\Final Demand\Total FD</t>
   </si>
 </sst>
 </file>
@@ -634,10 +646,10 @@
   <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="D20" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A26" sqref="A26"/>
+      <selection pane="bottomRight" activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -950,6 +962,9 @@
       <c r="D21" t="s">
         <v>84</v>
       </c>
+      <c r="E21" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
@@ -958,6 +973,9 @@
       <c r="D22" t="s">
         <v>89</v>
       </c>
+      <c r="E22" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
@@ -966,6 +984,9 @@
       <c r="D23" t="s">
         <v>92</v>
       </c>
+      <c r="E23" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
@@ -974,6 +995,9 @@
       <c r="D24" t="s">
         <v>84</v>
       </c>
+      <c r="E24" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
@@ -981,6 +1005,9 @@
       </c>
       <c r="D25" t="s">
         <v>90</v>
+      </c>
+      <c r="E25" t="s">
+        <v>97</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Plot for cumulative-met rec and plot for ratio cumulative-reserves
</commit_message>
<xml_diff>
--- a/Paths.xlsx
+++ b/Paths.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://polimi365-my.sharepoint.com/personal/10608728_polimi_it/Documents/Documenti/GitHub/GreenTechs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\carol\OneDrive\Documenti\GitHub\GreenTechs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="12" documentId="13_ncr:1_{FEEC7724-C12F-4C01-A047-E31064534AB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{350BB2CC-B1A9-4C55-AE67-DA7DC7A4BDF8}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B35F6DEC-C42D-4FC0-9817-DD8EE0EA8AA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="15260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="103">
   <si>
     <t>LR</t>
   </si>
@@ -319,6 +319,21 @@
   </si>
   <si>
     <t>C:\Users\matti\OneDrive - Politecnico di Milano\Documenti\GitHub\GreenTechs\Recycling\Met_rec_tech</t>
+  </si>
+  <si>
+    <t>C:\Users\carol\OneDrive\Documenti\GitHub\GreenTechs\Recycling\A2</t>
+  </si>
+  <si>
+    <t>C:\Users\carol\OneDrive\Documenti\GitHub\GreenTechs\Recycling\Met_rec_tech</t>
+  </si>
+  <si>
+    <t>C:\Users\carol\OneDrive\Documenti\GitHub\GreenTechs\Act</t>
+  </si>
+  <si>
+    <t>Baseline RR</t>
+  </si>
+  <si>
+    <t>C:\Users\carol\OneDrive\Documenti\GitHub\GreenTechs\Results\Baseline\RR</t>
   </si>
 </sst>
 </file>
@@ -643,13 +658,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E26"/>
+  <dimension ref="A1:E27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="D5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="D8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E21" sqref="E21"/>
+      <selection pane="bottomRight" activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -926,6 +941,9 @@
       <c r="A18" t="s">
         <v>90</v>
       </c>
+      <c r="D18" t="s">
+        <v>98</v>
+      </c>
       <c r="E18" t="s">
         <v>91</v>
       </c>
@@ -945,6 +963,9 @@
       <c r="A20" t="s">
         <v>96</v>
       </c>
+      <c r="D20" t="s">
+        <v>99</v>
+      </c>
       <c r="E20" t="s">
         <v>97</v>
       </c>
@@ -1008,8 +1029,19 @@
       <c r="A26" t="s">
         <v>92</v>
       </c>
+      <c r="D26" t="s">
+        <v>100</v>
+      </c>
       <c r="E26" t="s">
         <v>93</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>101</v>
+      </c>
+      <c r="D27" t="s">
+        <v>102</v>
       </c>
     </row>
   </sheetData>

</xml_diff>